<commit_message>
Update board statistics for June
</commit_message>
<xml_diff>
--- a/statistics_files/nekls_executive_board/2022/2022.06.next_search_catalog.xlsx
+++ b/statistics_files/nekls_executive_board/2022/2022.06.next_search_catalog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20382"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20387"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\GitHub\next_statistics\statistics_files\nekls_executive_board\2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8593BADA-CBC4-4D2E-BB4A-B4CFA9ABAD21}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33129796-E3C8-42A1-9CF2-3824EB5D4F0E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11295" xr2:uid="{4F58177C-A508-401B-B121-B6C236B4EE04}"/>
   </bookViews>
@@ -756,457 +756,799 @@
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
+      <c r="B3" s="5">
+        <v>36997</v>
+      </c>
+      <c r="C3" s="5">
+        <v>4954</v>
+      </c>
+      <c r="D3" s="5">
+        <v>6111</v>
+      </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
+      <c r="B4" s="7">
+        <v>17127</v>
+      </c>
+      <c r="C4" s="7">
+        <v>1880</v>
+      </c>
+      <c r="D4" s="7">
+        <v>2149</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
+      <c r="B5" s="5">
+        <v>59792</v>
+      </c>
+      <c r="C5" s="5">
+        <v>4154</v>
+      </c>
+      <c r="D5" s="5">
+        <v>5391</v>
+      </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
+      <c r="B6" s="7">
+        <v>1337</v>
+      </c>
+      <c r="C6" s="7">
+        <v>386</v>
+      </c>
+      <c r="D6" s="7">
+        <v>35</v>
+      </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
+      <c r="B7" s="5">
+        <v>35025</v>
+      </c>
+      <c r="C7" s="5">
+        <v>6276</v>
+      </c>
+      <c r="D7" s="5">
+        <v>5554</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
+      <c r="B8" s="7">
+        <v>4075</v>
+      </c>
+      <c r="C8" s="7">
+        <v>902</v>
+      </c>
+      <c r="D8" s="7">
+        <v>851</v>
+      </c>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
+      <c r="B9" s="5">
+        <v>4844</v>
+      </c>
+      <c r="C9" s="5">
+        <v>835</v>
+      </c>
+      <c r="D9" s="5">
+        <v>670</v>
+      </c>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
+      <c r="B10" s="7">
+        <v>1750</v>
+      </c>
+      <c r="C10" s="7">
+        <v>241</v>
+      </c>
+      <c r="D10" s="7">
+        <v>58</v>
+      </c>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
+      <c r="B11" s="5">
+        <v>345</v>
+      </c>
+      <c r="C11" s="5">
+        <v>186</v>
+      </c>
+      <c r="D11" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
+      <c r="B12" s="7">
+        <v>0</v>
+      </c>
+      <c r="C12" s="7">
+        <v>0</v>
+      </c>
+      <c r="D12" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
+      <c r="B13" s="9">
+        <v>879</v>
+      </c>
+      <c r="C13" s="9">
+        <v>245</v>
+      </c>
+      <c r="D13" s="9">
+        <v>212</v>
+      </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
+      <c r="B14" s="11">
+        <v>2353</v>
+      </c>
+      <c r="C14" s="11">
+        <v>1207</v>
+      </c>
+      <c r="D14" s="11">
+        <v>829</v>
+      </c>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
+      <c r="B15" s="9">
+        <v>4779</v>
+      </c>
+      <c r="C15" s="9">
+        <v>1703</v>
+      </c>
+      <c r="D15" s="9">
+        <v>833</v>
+      </c>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
+      <c r="B16" s="11">
+        <v>2933</v>
+      </c>
+      <c r="C16" s="11">
+        <v>1202</v>
+      </c>
+      <c r="D16" s="11">
+        <v>530</v>
+      </c>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
+      <c r="B17" s="5">
+        <v>1564</v>
+      </c>
+      <c r="C17" s="5">
+        <v>551</v>
+      </c>
+      <c r="D17" s="5">
+        <v>111</v>
+      </c>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
+      <c r="B18" s="7">
+        <v>14038</v>
+      </c>
+      <c r="C18" s="7">
+        <v>2132</v>
+      </c>
+      <c r="D18" s="7">
+        <v>2556</v>
+      </c>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
+      <c r="B19" s="5">
+        <v>2481</v>
+      </c>
+      <c r="C19" s="5">
+        <v>638</v>
+      </c>
+      <c r="D19" s="5">
+        <v>448</v>
+      </c>
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
+      <c r="B20" s="7">
+        <v>17510</v>
+      </c>
+      <c r="C20" s="7">
+        <v>1825</v>
+      </c>
+      <c r="D20" s="7">
+        <v>3064</v>
+      </c>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
+      <c r="B21" s="5">
+        <v>277</v>
+      </c>
+      <c r="C21" s="5">
+        <v>305</v>
+      </c>
+      <c r="D21" s="5">
+        <v>12</v>
+      </c>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
+      <c r="B22" s="7">
+        <v>15261</v>
+      </c>
+      <c r="C22" s="7">
+        <v>1757</v>
+      </c>
+      <c r="D22" s="7">
+        <v>2340</v>
+      </c>
     </row>
     <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
+      <c r="B23" s="5">
+        <v>949</v>
+      </c>
+      <c r="C23" s="5">
+        <v>391</v>
+      </c>
+      <c r="D23" s="5">
+        <v>140</v>
+      </c>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
+      <c r="B24" s="7">
+        <v>14597</v>
+      </c>
+      <c r="C24" s="7">
+        <v>2581</v>
+      </c>
+      <c r="D24" s="7">
+        <v>2605</v>
+      </c>
     </row>
     <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
+      <c r="B25" s="5">
+        <v>56062</v>
+      </c>
+      <c r="C25" s="5">
+        <v>6579</v>
+      </c>
+      <c r="D25" s="5">
+        <v>6348</v>
+      </c>
     </row>
     <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
+      <c r="B26" s="7">
+        <v>4225</v>
+      </c>
+      <c r="C26" s="7">
+        <v>1309</v>
+      </c>
+      <c r="D26" s="7">
+        <v>554</v>
+      </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
+      <c r="B27" s="5">
+        <v>0</v>
+      </c>
+      <c r="C27" s="5">
+        <v>0</v>
+      </c>
+      <c r="D27" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
+      <c r="B28" s="7">
+        <v>4785</v>
+      </c>
+      <c r="C28" s="7">
+        <v>894</v>
+      </c>
+      <c r="D28" s="7">
+        <v>991</v>
+      </c>
     </row>
     <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
+      <c r="B29" s="5">
+        <v>2234</v>
+      </c>
+      <c r="C29" s="5">
+        <v>262</v>
+      </c>
+      <c r="D29" s="5">
+        <v>449</v>
+      </c>
     </row>
     <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
+      <c r="B30" s="7">
+        <v>12903</v>
+      </c>
+      <c r="C30" s="7">
+        <v>2310</v>
+      </c>
+      <c r="D30" s="7">
+        <v>1946</v>
+      </c>
     </row>
     <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
+      <c r="B31" s="5">
+        <v>423</v>
+      </c>
+      <c r="C31" s="5">
+        <v>223</v>
+      </c>
+      <c r="D31" s="5">
+        <v>173</v>
+      </c>
     </row>
     <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
+      <c r="B32" s="7">
+        <v>1893</v>
+      </c>
+      <c r="C32" s="7">
+        <v>1325</v>
+      </c>
+      <c r="D32" s="7">
+        <v>229</v>
+      </c>
     </row>
     <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
+      <c r="B33" s="5">
+        <v>12452</v>
+      </c>
+      <c r="C33" s="5">
+        <v>2564</v>
+      </c>
+      <c r="D33" s="5">
+        <v>2279</v>
+      </c>
     </row>
     <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
+      <c r="B34" s="7">
+        <v>9547</v>
+      </c>
+      <c r="C34" s="7">
+        <v>2177</v>
+      </c>
+      <c r="D34" s="7">
+        <v>2399</v>
+      </c>
     </row>
     <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
+      <c r="B35" s="5">
+        <v>5404</v>
+      </c>
+      <c r="C35" s="5">
+        <v>631</v>
+      </c>
+      <c r="D35" s="5">
+        <v>1185</v>
+      </c>
     </row>
     <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
+      <c r="B36" s="7">
+        <v>42528</v>
+      </c>
+      <c r="C36" s="7">
+        <v>4554</v>
+      </c>
+      <c r="D36" s="7">
+        <v>4581</v>
+      </c>
     </row>
     <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
+      <c r="B37" s="5">
+        <v>6978</v>
+      </c>
+      <c r="C37" s="5">
+        <v>2235</v>
+      </c>
+      <c r="D37" s="5">
+        <v>1105</v>
+      </c>
     </row>
     <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
+      <c r="B38" s="7">
+        <v>15507</v>
+      </c>
+      <c r="C38" s="7">
+        <v>1647</v>
+      </c>
+      <c r="D38" s="7">
+        <v>2403</v>
+      </c>
     </row>
     <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
+      <c r="B39" s="5">
+        <v>759</v>
+      </c>
+      <c r="C39" s="5">
+        <v>610</v>
+      </c>
+      <c r="D39" s="5">
+        <v>129</v>
+      </c>
     </row>
     <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
+      <c r="B40" s="7">
+        <v>1351</v>
+      </c>
+      <c r="C40" s="7">
+        <v>210</v>
+      </c>
+      <c r="D40" s="7">
+        <v>753</v>
+      </c>
     </row>
     <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B41" s="13"/>
-      <c r="C41" s="13"/>
-      <c r="D41" s="13"/>
+      <c r="B41" s="13">
+        <v>1827</v>
+      </c>
+      <c r="C41" s="13">
+        <v>234</v>
+      </c>
+      <c r="D41" s="13">
+        <v>130</v>
+      </c>
     </row>
     <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="B42" s="15"/>
-      <c r="C42" s="15"/>
-      <c r="D42" s="15"/>
+      <c r="B42" s="15">
+        <v>7719</v>
+      </c>
+      <c r="C42" s="15">
+        <v>248</v>
+      </c>
+      <c r="D42" s="15">
+        <v>192</v>
+      </c>
     </row>
     <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B43" s="13"/>
-      <c r="C43" s="13"/>
-      <c r="D43" s="13"/>
+      <c r="B43" s="13">
+        <v>240</v>
+      </c>
+      <c r="C43" s="13">
+        <v>102</v>
+      </c>
+      <c r="D43" s="13">
+        <v>72</v>
+      </c>
     </row>
     <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="B44" s="15"/>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15"/>
+      <c r="B44" s="15">
+        <v>551</v>
+      </c>
+      <c r="C44" s="15">
+        <v>48</v>
+      </c>
+      <c r="D44" s="15">
+        <v>22</v>
+      </c>
     </row>
     <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B45" s="13"/>
-      <c r="C45" s="13"/>
-      <c r="D45" s="13"/>
+      <c r="B45" s="13">
+        <v>1743</v>
+      </c>
+      <c r="C45" s="13">
+        <v>159</v>
+      </c>
+      <c r="D45" s="13">
+        <v>73</v>
+      </c>
     </row>
     <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B46" s="7"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="7"/>
+      <c r="B46" s="7">
+        <v>2729</v>
+      </c>
+      <c r="C46" s="7">
+        <v>768</v>
+      </c>
+      <c r="D46" s="7">
+        <v>401</v>
+      </c>
     </row>
     <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
+      <c r="B47" s="5">
+        <v>9918</v>
+      </c>
+      <c r="C47" s="5">
+        <v>2619</v>
+      </c>
+      <c r="D47" s="5">
+        <v>2001</v>
+      </c>
     </row>
     <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="7"/>
+      <c r="B48" s="7">
+        <v>26083</v>
+      </c>
+      <c r="C48" s="7">
+        <v>2566</v>
+      </c>
+      <c r="D48" s="7">
+        <v>3867</v>
+      </c>
     </row>
     <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B49" s="5"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
+      <c r="B49" s="5">
+        <v>12412</v>
+      </c>
+      <c r="C49" s="5">
+        <v>2710</v>
+      </c>
+      <c r="D49" s="5">
+        <v>902</v>
+      </c>
     </row>
     <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B50" s="7"/>
-      <c r="C50" s="7"/>
-      <c r="D50" s="7"/>
+      <c r="B50" s="7">
+        <v>8730</v>
+      </c>
+      <c r="C50" s="7">
+        <v>875</v>
+      </c>
+      <c r="D50" s="7">
+        <v>1418</v>
+      </c>
     </row>
     <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B51" s="5"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
+      <c r="B51" s="5">
+        <v>21707</v>
+      </c>
+      <c r="C51" s="5">
+        <v>2443</v>
+      </c>
+      <c r="D51" s="5">
+        <v>2637</v>
+      </c>
     </row>
     <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B52" s="7"/>
-      <c r="C52" s="7"/>
-      <c r="D52" s="7"/>
+      <c r="B52" s="7">
+        <v>3183</v>
+      </c>
+      <c r="C52" s="7">
+        <v>380</v>
+      </c>
+      <c r="D52" s="7">
+        <v>689</v>
+      </c>
     </row>
     <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B53" s="5"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
+      <c r="B53" s="5">
+        <v>11102</v>
+      </c>
+      <c r="C53" s="5">
+        <v>2274</v>
+      </c>
+      <c r="D53" s="5">
+        <v>2021</v>
+      </c>
     </row>
     <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B54" s="7"/>
-      <c r="C54" s="7"/>
-      <c r="D54" s="7"/>
+      <c r="B54" s="7">
+        <v>1882</v>
+      </c>
+      <c r="C54" s="7">
+        <v>565</v>
+      </c>
+      <c r="D54" s="7">
+        <v>972</v>
+      </c>
     </row>
     <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B55" s="5"/>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
+      <c r="B55" s="5">
+        <v>1580</v>
+      </c>
+      <c r="C55" s="5">
+        <v>1131</v>
+      </c>
+      <c r="D55" s="5">
+        <v>192</v>
+      </c>
     </row>
     <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B56" s="7"/>
-      <c r="C56" s="7"/>
-      <c r="D56" s="7"/>
+      <c r="B56" s="7">
+        <v>2978</v>
+      </c>
+      <c r="C56" s="7">
+        <v>864</v>
+      </c>
+      <c r="D56" s="7">
+        <v>1037</v>
+      </c>
     </row>
     <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="B57" s="17"/>
-      <c r="C57" s="17"/>
-      <c r="D57" s="17"/>
+      <c r="B57" s="17">
+        <v>10944</v>
+      </c>
+      <c r="C57" s="17">
+        <v>4357</v>
+      </c>
+      <c r="D57" s="17">
+        <v>2404</v>
+      </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="B58" s="19"/>
-      <c r="C58" s="19"/>
-      <c r="D58" s="19"/>
+      <c r="B58" s="19">
+        <v>12080</v>
+      </c>
+      <c r="C58" s="19">
+        <v>791</v>
+      </c>
+      <c r="D58" s="19">
+        <v>489</v>
+      </c>
     </row>
     <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="B59" s="21"/>
-      <c r="C59" s="21"/>
-      <c r="D59" s="21"/>
+      <c r="B59" s="21">
+        <v>530348</v>
+      </c>
+      <c r="C59" s="21">
+        <v>79867</v>
+      </c>
+      <c r="D59" s="21">
+        <v>76650</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A2:D59" xr:uid="{6CA45A21-3256-46F4-A196-E6610455B173}"/>

</xml_diff>